<commit_message>
Excel file code helper
</commit_message>
<xml_diff>
--- a/assets/Testing/code helper.xlsx
+++ b/assets/Testing/code helper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reeveschragger/Documents/Bootcamp/Challenges/BC06-02-Weather-Dashboard/assets/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73B5439-1C44-E847-A4BE-36975A142AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964C1BD3-184D-AB40-96B3-A7E8674D8BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16460" activeTab="2" xr2:uid="{77A161DF-F974-AC46-AA74-EF0FB37B311E}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="2" xr2:uid="{77A161DF-F974-AC46-AA74-EF0FB37B311E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="112">
   <si>
     <t>dt</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>wind_deg</t>
+  </si>
+  <si>
+    <t>weather</t>
   </si>
   <si>
     <t xml:space="preserve"> id</t>
@@ -809,18 +812,18 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" t="str">
         <f>"&lt;div class="""&amp;B2 &amp; """ id="""</f>
@@ -843,10 +846,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C18" si="0">"&lt;div class="""&amp;B3 &amp; """ id="""</f>
@@ -869,10 +872,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -895,10 +898,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -921,10 +924,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -947,10 +950,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -973,10 +976,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -999,10 +1002,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -1025,10 +1028,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -1051,10 +1054,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -1077,10 +1080,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -1103,10 +1106,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -1129,10 +1132,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -1155,17 +1158,17 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>&lt;div class="today-info" id="</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
@@ -1181,17 +1184,17 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>&lt;div class="today-info" id="</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
@@ -1202,22 +1205,22 @@
         <v>&lt;div class="today-info" id="mainToday"&gt;Clear&lt;/div&gt;</v>
       </c>
       <c r="L16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>&lt;div class="today-info" id="</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
@@ -1228,22 +1231,22 @@
         <v>&lt;div class="today-info" id="descriptionToday"&gt;clear sky&lt;/div&gt;</v>
       </c>
       <c r="L17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>&lt;div class="today-info" id="</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
@@ -1254,19 +1257,19 @@
         <v>&lt;div class="today-info" id="iconToday"&gt;01n&lt;/div&gt;</v>
       </c>
       <c r="L18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="43" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D21" t="str">
         <f>D2</f>
         <v>dt</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G21" t="str">
         <f>"#"&amp;D21&amp;"Today::before{content: '" &amp;E21&amp;": ';}"</f>
@@ -1309,7 +1312,7 @@
         <v>temp</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="5"/>
@@ -1322,7 +1325,7 @@
         <v>feels_like</v>
       </c>
       <c r="E25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="5"/>
@@ -1363,7 +1366,7 @@
         <v>dew_point</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="5"/>
@@ -1376,7 +1379,7 @@
         <v>uvi</v>
       </c>
       <c r="E29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="5"/>
@@ -1417,7 +1420,7 @@
         <v>wind_speed</v>
       </c>
       <c r="E32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="5"/>
@@ -1430,7 +1433,7 @@
         <v>wind_deg</v>
       </c>
       <c r="E33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="5"/>
@@ -1507,36 +1510,36 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" t="str">
         <f>A$1 &amp; ":'" &amp; (A2) &amp;"', "</f>
@@ -1568,16 +1571,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F37" si="1">A$1 &amp; ":'" &amp; (A3) &amp;"', "</f>
@@ -1606,19 +1609,19 @@
     </row>
     <row r="4" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -1647,7 +1650,7 @@
     </row>
     <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -1676,19 +1679,19 @@
     </row>
     <row r="6" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
@@ -1717,19 +1720,19 @@
     </row>
     <row r="7" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
@@ -1758,7 +1761,7 @@
     </row>
     <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -1787,19 +1790,19 @@
     </row>
     <row r="9" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -1828,19 +1831,19 @@
     </row>
     <row r="10" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -1872,16 +1875,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
@@ -1913,16 +1916,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -1951,7 +1954,7 @@
     </row>
     <row r="13" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
@@ -1983,16 +1986,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
@@ -2024,16 +2027,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
@@ -2062,19 +2065,19 @@
     </row>
     <row r="16" spans="1:13" ht="62" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
@@ -2103,19 +2106,19 @@
     </row>
     <row r="17" spans="1:13" ht="62" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
@@ -2147,16 +2150,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
@@ -2185,19 +2188,19 @@
     </row>
     <row r="19" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="D19" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
@@ -2226,19 +2229,19 @@
     </row>
     <row r="20" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
@@ -2267,7 +2270,7 @@
     </row>
     <row r="21" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
@@ -2296,19 +2299,19 @@
     </row>
     <row r="22" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
@@ -2337,19 +2340,19 @@
     </row>
     <row r="23" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
@@ -2378,19 +2381,19 @@
     </row>
     <row r="24" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
@@ -2448,19 +2451,19 @@
     </row>
     <row r="26" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>
@@ -2489,7 +2492,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="1"/>
@@ -2518,19 +2521,19 @@
     </row>
     <row r="28" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="1"/>
@@ -2559,19 +2562,19 @@
     </row>
     <row r="29" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="1"/>
@@ -2600,19 +2603,19 @@
     </row>
     <row r="30" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="1"/>
@@ -2641,19 +2644,19 @@
     </row>
     <row r="31" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="1"/>
@@ -2682,7 +2685,7 @@
     </row>
     <row r="32" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="1"/>
@@ -2711,19 +2714,19 @@
     </row>
     <row r="33" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="1"/>
@@ -2752,19 +2755,19 @@
     </row>
     <row r="34" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="D34" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="1"/>
@@ -2793,7 +2796,7 @@
     </row>
     <row r="35" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="1"/>
@@ -2822,19 +2825,19 @@
     </row>
     <row r="36" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="1"/>
@@ -2863,19 +2866,19 @@
     </row>
     <row r="37" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="D37" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="1"/>
@@ -2914,8 +2917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806F19DD-A6CB-604C-A740-8191C564D162}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M38"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2935,31 +2938,31 @@
   <sheetData>
     <row r="1" spans="1:18" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="22" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2994,16 +2997,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:J37" si="1">A$1 &amp; ":'" &amp; (A3) &amp;"', "</f>
@@ -3032,10 +3035,10 @@
     </row>
     <row r="4" spans="1:18" ht="22" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -3067,7 +3070,7 @@
     </row>
     <row r="5" spans="1:18" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -3096,10 +3099,10 @@
     </row>
     <row r="6" spans="1:18" ht="22" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -3131,10 +3134,10 @@
     </row>
     <row r="7" spans="1:18" ht="22" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -3166,7 +3169,7 @@
     </row>
     <row r="8" spans="1:18" ht="21" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -3195,10 +3198,10 @@
     </row>
     <row r="9" spans="1:18" ht="22" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -3230,10 +3233,10 @@
     </row>
     <row r="10" spans="1:18" ht="22" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -3268,16 +3271,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
@@ -3309,16 +3312,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -3347,7 +3350,7 @@
     </row>
     <row r="13" spans="1:18" ht="21" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
@@ -3379,16 +3382,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
@@ -3420,16 +3423,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
@@ -3458,19 +3461,19 @@
     </row>
     <row r="16" spans="1:18" ht="62" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
@@ -3499,19 +3502,19 @@
     </row>
     <row r="17" spans="1:13" ht="62" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
@@ -3543,16 +3546,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
@@ -3581,19 +3584,19 @@
     </row>
     <row r="19" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="D19" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
@@ -3622,19 +3625,19 @@
     </row>
     <row r="20" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
@@ -3663,7 +3666,7 @@
     </row>
     <row r="21" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
@@ -3692,19 +3695,19 @@
     </row>
     <row r="22" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
@@ -3733,19 +3736,19 @@
     </row>
     <row r="23" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
@@ -3774,19 +3777,19 @@
     </row>
     <row r="24" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
@@ -3844,19 +3847,19 @@
     </row>
     <row r="26" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>
@@ -3885,11 +3888,11 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">parameter:'weather (more info Weather condition codes)', </v>
+        <v xml:space="preserve">parameter:'weather', </v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
@@ -3909,15 +3912,15 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" si="2"/>
-        <v>weather (more info Weather condition codes):{parameter:'weather (more info Weather condition codes)', description:'', standard:'', metric:'', imperial:'', },</v>
+        <v>weather:{parameter:'weather', description:'', standard:'', metric:'', imperial:'', },</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -3949,10 +3952,10 @@
     </row>
     <row r="29" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -3984,10 +3987,10 @@
     </row>
     <row r="30" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -4019,10 +4022,10 @@
     </row>
     <row r="31" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -4054,7 +4057,7 @@
     </row>
     <row r="32" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="1"/>
@@ -4083,19 +4086,19 @@
     </row>
     <row r="33" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="1"/>
@@ -4124,19 +4127,19 @@
     </row>
     <row r="34" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="D34" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="1"/>
@@ -4165,7 +4168,7 @@
     </row>
     <row r="35" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="1"/>
@@ -4194,19 +4197,19 @@
     </row>
     <row r="36" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="1"/>
@@ -4235,19 +4238,19 @@
     </row>
     <row r="37" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="D37" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="1"/>
@@ -4276,7 +4279,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M38" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bring concepts from testing to main
</commit_message>
<xml_diff>
--- a/assets/Testing/code helper.xlsx
+++ b/assets/Testing/code helper.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reeveschragger/Documents/Bootcamp/Challenges/BC06-02-Weather-Dashboard/assets/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964C1BD3-184D-AB40-96B3-A7E8674D8BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CAFE7E-653D-624F-A7ED-B586A2EF39CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="2" xr2:uid="{77A161DF-F974-AC46-AA74-EF0FB37B311E}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="3" xr2:uid="{77A161DF-F974-AC46-AA74-EF0FB37B311E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="units_try1" sheetId="2" r:id="rId2"/>
     <sheet name="units_try2" sheetId="3" r:id="rId3"/>
+    <sheet name="units_try3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">units_try3!$A$1:$S$38</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="112">
   <si>
     <t>dt</t>
   </si>
@@ -1546,7 +1550,7 @@
         <v xml:space="preserve">Parameter:'id', </v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:K2" si="0">B$1 &amp; ":'" &amp; (B2) &amp;"', "</f>
+        <f t="shared" ref="G2:J2" si="0">B$1 &amp; ":'" &amp; (B2) &amp;"', "</f>
         <v xml:space="preserve">Description:'City identification', </v>
       </c>
       <c r="H2" t="str">
@@ -2917,8 +2921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806F19DD-A6CB-604C-A740-8191C564D162}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A12" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4288,4 +4292,1383 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE5867C-ED1E-974D-873D-48CABD489485}">
+  <dimension ref="A1:S38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.6640625" style="11" customWidth="1"/>
+    <col min="4" max="6" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" t="str">
+        <f>B$1 &amp; ":'" &amp; (B2) &amp;"', "</f>
+        <v xml:space="preserve">parameter:'id', </v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:K17" si="0">C$1 &amp; ":'" &amp; (C2) &amp;"', "</f>
+        <v xml:space="preserve">description:'City identification', </v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N2" t="str">
+        <f>IF(B2="","", B2 &amp; ":{"&amp;_xlfn.CONCAT(G2:L2) &amp; "},")</f>
+        <v>id:{parameter:'id', description:'City identification', standard:'', metric:'', imperial:'', },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:K37" si="1">B$1 &amp; ":'" &amp; (B3) &amp;"', "</f>
+        <v xml:space="preserve">parameter:'dt', </v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'Data receiving time', </v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'unix, UTC', </v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'unix, UTC', </v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'unix, UTC', </v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N38" si="2">IF(B3="","", B3 &amp; ":{"&amp;_xlfn.CONCAT(G3:L3) &amp; "},")</f>
+        <v>dt:{parameter:'dt', description:'Data receiving time', standard:'unix, UTC', metric:'unix, UTC', imperial:'unix, UTC', },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'name', </v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'City name', </v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="2"/>
+        <v>name:{parameter:'name', description:'City name', standard:'', metric:'', imperial:'', },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="21" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="str">
+        <f>B$1 &amp; ":'" &amp; (A5) &amp;"', "</f>
+        <v xml:space="preserve">parameter:'coord', </v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'', </v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'lat', </v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'City geo location, latitude', </v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="2"/>
+        <v>lat:{parameter:'lat', description:'City geo location, latitude', standard:'', metric:'', imperial:'', },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'lon', </v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'City geo location, longitude', </v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="2"/>
+        <v>lon:{parameter:'lon', description:'City geo location, longitude', standard:'', metric:'', imperial:'', },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="21" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="str">
+        <f>B$1 &amp; ":'" &amp; (A8) &amp;"', "</f>
+        <v xml:space="preserve">parameter:'sys', </v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'', </v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'message', </v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'System parameter, do not use it', </v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="2"/>
+        <v>message:{parameter:'message', description:'System parameter, do not use it', standard:'', metric:'', imperial:'', },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'country', </v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'Country code (GB, JP etc.)', </v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="2"/>
+        <v>country:{parameter:'country', description:'Country code (GB, JP etc.)', standard:'', metric:'', imperial:'', },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'sunrise', </v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'Sunrise time', </v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'unix, UTC', </v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'unix, UTC', </v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'unix, UTC', </v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="2"/>
+        <v>sunrise:{parameter:'sunrise', description:'Sunrise time', standard:'unix, UTC', metric:'unix, UTC', imperial:'unix, UTC', },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'sunset', </v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'Sunset time', </v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'unix, UTC', </v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'unix, UTC', </v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'unix, UTC', </v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="2"/>
+        <v>sunset:{parameter:'sunset', description:'Sunset time', standard:'unix, UTC', metric:'unix, UTC', imperial:'unix, UTC', },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="21" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="str">
+        <f>B$1 &amp; ":'" &amp; (A13) &amp;"', "</f>
+        <v xml:space="preserve">parameter:'main', </v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'', </v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'temp', </v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'Temperature', </v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'°K', </v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'°C', </v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'°F', </v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="2"/>
+        <v>temp:{parameter:'temp', description:'Temperature', standard:'°K', metric:'°C', imperial:'°F', },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="22" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'humidity', </v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'Humidity', </v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'%', </v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'%', </v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'%', </v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="2"/>
+        <v>humidity:{parameter:'humidity', description:'Humidity', standard:'%', metric:'%', imperial:'%', },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="62" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'temp_min', </v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'Minimum temperature at the moment. This is deviation from current temp that is possible for large cities and megalopolises geographically expanded (use these parameter optionally)', </v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'°K', </v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'°C', </v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'°F', </v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="2"/>
+        <v>temp_min:{parameter:'temp_min', description:'Minimum temperature at the moment. This is deviation from current temp that is possible for large cities and megalopolises geographically expanded (use these parameter optionally)', standard:'°K', metric:'°C', imperial:'°F', },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="62" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'temp_max', </v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">description:'Maximum temperature at the moment. This is deviation from current temp that is possible for large cities and megalopolises geographically expanded (use these parameter optionally)', </v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">standard:'°K', </v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">metric:'°C', </v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">imperial:'°F', </v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="2"/>
+        <v>temp_max:{parameter:'temp_max', description:'Maximum temperature at the moment. This is deviation from current temp that is possible for large cities and megalopolises geographically expanded (use these parameter optionally)', standard:'°K', metric:'°C', imperial:'°F', },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'pressure', </v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Atmospheric pressure (on the sea level, if there is no sea_level or grnd_level data)', </v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'hPa', </v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'hPa', </v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'hPa', </v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="2"/>
+        <v>pressure:{parameter:'pressure', description:'Atmospheric pressure (on the sea level, if there is no sea_level or grnd_level data)', standard:'hPa', metric:'hPa', imperial:'hPa', },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'sea_level', </v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Atmospheric pressure on the sea level', </v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'hPa', </v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'hPa', </v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'hPa', </v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="2"/>
+        <v>sea_level:{parameter:'sea_level', description:'Atmospheric pressure on the sea level', standard:'hPa', metric:'hPa', imperial:'hPa', },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'grnd_level', </v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Atmospheric pressure on the ground level', </v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'hPa', </v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'hPa', </v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'hPa', </v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="2"/>
+        <v>grnd_level:{parameter:'grnd_level', description:'Atmospheric pressure on the ground level', standard:'hPa', metric:'hPa', imperial:'hPa', },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" t="str">
+        <f>B$1 &amp; ":'" &amp; (A21) &amp;"', "</f>
+        <v xml:space="preserve">parameter:'wind', </v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'', </v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'speed', </v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Wind speed', </v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'m/s', </v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'m/s', </v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'m/hr', </v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="2"/>
+        <v>speed:{parameter:'speed', description:'Wind speed', standard:'m/s', metric:'m/s', imperial:'m/hr', },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'deg', </v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Wind direction', </v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'° (meteorological)', </v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'° (meteorological)', </v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'° (meteorological)', </v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="2"/>
+        <v>deg:{parameter:'deg', description:'Wind direction', standard:'° (meteorological)', metric:'° (meteorological)', imperial:'° (meteorological)', },</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'gust', </v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Wind gust', </v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'m/s', </v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'m/s', </v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'m/hr', </v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="2"/>
+        <v>gust:{parameter:'gust', description:'Wind gust', standard:'m/s', metric:'m/s', imperial:'m/hr', },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" t="str">
+        <f>B$1 &amp; ":'" &amp; (A25) &amp;"', "</f>
+        <v xml:space="preserve">parameter:'clouds', </v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'', </v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'all', </v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Cloudiness', </v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'%', </v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'%', </v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'%', </v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="2"/>
+        <v>all:{parameter:'all', description:'Cloudiness', standard:'%', metric:'%', imperial:'%', },</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="str">
+        <f>B$1 &amp; ":'" &amp; (A27) &amp;"', "</f>
+        <v xml:space="preserve">parameter:'weather', </v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'', </v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'id', </v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Weather condition id', </v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="2"/>
+        <v>id:{parameter:'id', description:'Weather condition id', standard:'', metric:'', imperial:'', },</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'main', </v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Group of weather parameters (Rain, Snow, Extreme etc.)', </v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="2"/>
+        <v>main:{parameter:'main', description:'Group of weather parameters (Rain, Snow, Extreme etc.)', standard:'', metric:'', imperial:'', },</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B30" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'description', </v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Weather condition within the group', </v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="2"/>
+        <v>description:{parameter:'description', description:'Weather condition within the group', standard:'', metric:'', imperial:'', },</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'icon', </v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Weather icon id', </v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="2"/>
+        <v>icon:{parameter:'icon', description:'Weather icon id', standard:'', metric:'', imperial:'', },</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" t="str">
+        <f>B$1 &amp; ":'" &amp; (A32) &amp;"', "</f>
+        <v xml:space="preserve">parameter:'rain', </v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'', </v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B33" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'1h', </v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Precipitation volume for last hour', </v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'mm', </v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'mm', </v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'mm', </v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="2"/>
+        <v>1h:{parameter:'1h', description:'Precipitation volume for last hour', standard:'mm', metric:'mm', imperial:'mm', },</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B34" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'3h', </v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Precipitation volume for last 3 hours', </v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'mm', </v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'mm', </v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'mm', </v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="2"/>
+        <v>3h:{parameter:'3h', description:'Precipitation volume for last 3 hours', standard:'mm', metric:'mm', imperial:'mm', },</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" t="str">
+        <f>B$1 &amp; ":'" &amp; (A35) &amp;"', "</f>
+        <v xml:space="preserve">parameter:'snow', </v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'', </v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'', </v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'', </v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'', </v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B36" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'1h', </v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Snow volume for last hour', </v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'mm', </v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'mm', </v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'mm', </v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="2"/>
+        <v>1h:{parameter:'1h', description:'Snow volume for last hour', standard:'mm', metric:'mm', imperial:'mm', },</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="B37" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">parameter:'3h', </v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">description:'Snow volume for last 3 hours', </v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">standard:'mm', </v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">metric:'mm', </v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">imperial:'mm', </v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="2"/>
+        <v>3h:{parameter:'3h', description:'Snow volume for last 3 hours', standard:'mm', metric:'mm', imperial:'mm', },</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N38" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:S38" xr:uid="{FEE5867C-ED1E-974D-873D-48CABD489485}"/>
+  <hyperlinks>
+    <hyperlink ref="A27" r:id="rId1" display="https://openweathermap.org/weather-conditions" xr:uid="{7F6D9F15-168B-D947-B58F-666C4AB1D0D5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>